<commit_message>
Fixed a bug in the .xlsx file that ruined the tab-delimited file
</commit_message>
<xml_diff>
--- a/data/Survey-Data.xlsx
+++ b/data/Survey-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmalt\Desktop\MCB536-Files\homework-assignments\tfcb-homework02\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91B194C-CEDD-43CD-9B9A-DC178217554F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADACC652-6FCB-4090-90D3-05C72E9312F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="460" windowWidth="17080" windowHeight="10090" tabRatio="481" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1110" yWindow="110" windowWidth="17080" windowHeight="10090" tabRatio="481" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined-data" sheetId="1" r:id="rId1"/>
@@ -147,7 +147,7 @@
     <t>OL</t>
   </si>
   <si>
-    <t>Field season</t>
+    <t>Field-season</t>
   </si>
 </sst>
 </file>
@@ -676,7 +676,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -720,7 +720,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -745,7 +745,7 @@
   <dimension ref="C3:AC52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="25" x14ac:dyDescent="0.5"/>

</xml_diff>